<commit_message>
Updated results after running the code again
</commit_message>
<xml_diff>
--- a/data/interim/Impacts_recipes.xlsx
+++ b/data/interim/Impacts_recipes.xlsx
@@ -441,17 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>impacts_recipe_1</t>
+          <t>Recipe 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>impacts_recipe_2</t>
+          <t>Recipe 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>impacts_recipe_3</t>
+          <t>Recipe 3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates before the final delivery
</commit_message>
<xml_diff>
--- a/data/interim/Impacts_recipes.xlsx
+++ b/data/interim/Impacts_recipes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,32 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Recipe Lomo Saltado with beef</t>
+          <t>Recipe Chicken in creme freice</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Recipe Lomo Saltado with chicken</t>
+          <t>Recipe Chilli con carne</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Recipe Lomo Saltado with chickpeas</t>
+          <t>Recipe Kylling og søtpotet</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Recipe Lomo Saltado with mushrooms</t>
+          <t>Recipe Meeeeeat</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recipe Lomo Saltado with salmon</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Recipe Lomo Saltado with tofu</t>
+          <t>Recipe Porrige</t>
         </is>
       </c>
     </row>
@@ -477,22 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13.7190236</v>
+        <v>7.598879200000001</v>
       </c>
       <c r="C2" t="n">
-        <v>6.9636386</v>
+        <v>18.3786192</v>
       </c>
       <c r="D2" t="n">
-        <v>8.8705436</v>
+        <v>5.865119999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>4.4898036</v>
+        <v>39.58889000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>5.6031886</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5.513553600000001</v>
+        <v>7.896140000000001</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.0133508</v>
+        <v>2.4108816</v>
       </c>
       <c r="C3" t="n">
-        <v>1.5405158</v>
+        <v>5.2816516</v>
       </c>
       <c r="D3" t="n">
-        <v>2.4227608</v>
+        <v>1.87952</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7474508</v>
+        <v>10.18122</v>
       </c>
       <c r="F3" t="n">
-        <v>1.0300058</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1.0177208</v>
+        <v>2.61902</v>
       </c>
     </row>
     <row r="4">
@@ -527,7 +516,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>76.48186</v>
+        <v>2.1335</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -536,14 +525,11 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>304.88735</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -552,22 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8.503787599999999</v>
+        <v>2.7094856</v>
       </c>
       <c r="C5" t="n">
-        <v>2.2529976</v>
+        <v>7.0928056</v>
       </c>
       <c r="D5" t="n">
-        <v>1.1123126</v>
+        <v>2.27488</v>
       </c>
       <c r="E5" t="n">
-        <v>1.0977526</v>
+        <v>29.97520999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>1.3402676</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.5331876</v>
+        <v>0.5462349999999999</v>
       </c>
     </row>
     <row r="6">
@@ -577,21 +560,18 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8544899999999999</v>
+        <v>1.50024</v>
       </c>
       <c r="C6" t="n">
-        <v>0.807625</v>
+        <v>1.42</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1.42</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>3.46772</v>
       </c>
       <c r="F6" t="n">
-        <v>0.372645</v>
-      </c>
-      <c r="G6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -602,22 +582,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>20.7405214</v>
+        <v>2.0526036</v>
       </c>
       <c r="C7" t="n">
-        <v>3.1247414</v>
+        <v>6.511263600000001</v>
       </c>
       <c r="D7" t="n">
-        <v>3.3144764</v>
+        <v>1.28196</v>
       </c>
       <c r="E7" t="n">
-        <v>2.8981514</v>
+        <v>72.69932</v>
       </c>
       <c r="F7" t="n">
-        <v>4.456071400000001</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3.0442064</v>
+        <v>2.81877</v>
       </c>
     </row>
     <row r="8">
@@ -627,22 +604,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6889980000000001</v>
+        <v>0.5631828</v>
       </c>
       <c r="C8" t="n">
-        <v>0.311803</v>
+        <v>0.6547527999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>0.111603</v>
+        <v>0.36236</v>
       </c>
       <c r="E8" t="n">
-        <v>0.138903</v>
+        <v>2.36005</v>
       </c>
       <c r="F8" t="n">
-        <v>0.120703</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.4728730000000001</v>
+        <v>0.35745</v>
       </c>
     </row>
     <row r="9">
@@ -652,22 +626,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.3578433999999999</v>
+        <v>0.4871432000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3259933999999999</v>
+        <v>0.6006731999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2440934</v>
+        <v>0.45712</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2750333999999999</v>
+        <v>1.01004</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2509184</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.2809483999999999</v>
+        <v>0.516635</v>
       </c>
     </row>
     <row r="10">
@@ -677,22 +648,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3899102</v>
+        <v>0.3798696</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3739852000000001</v>
+        <v>1.0533096</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4381402</v>
+        <v>0.30928</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2961802000000001</v>
+        <v>0.74295</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3052802000000001</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.3580602</v>
+        <v>0.39381</v>
       </c>
     </row>
     <row r="11">
@@ -702,22 +670,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1350142</v>
+        <v>0.2819676</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1409292</v>
+        <v>0.2299776</v>
       </c>
       <c r="D11" t="n">
-        <v>0.07813920000000001</v>
+        <v>0.22036</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06721920000000001</v>
+        <v>0.4837</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0785942</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.1832442</v>
+        <v>0.442385</v>
       </c>
     </row>
     <row r="12">
@@ -727,22 +692,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.107303026</v>
+        <v>0.07090242000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>0.050473526</v>
+        <v>0.09367762000000002</v>
       </c>
       <c r="D12" t="n">
-        <v>0.029880226</v>
+        <v>0.06318120000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>0.023592126</v>
+        <v>0.3644722</v>
       </c>
       <c r="F12" t="n">
-        <v>0.032551076</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.024019826</v>
+        <v>0.02128775</v>
       </c>
     </row>
     <row r="13">
@@ -752,22 +714,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.103184908</v>
+        <v>0.036352752</v>
       </c>
       <c r="C13" t="n">
-        <v>0.035890408</v>
+        <v>0.070164752</v>
       </c>
       <c r="D13" t="n">
-        <v>0.029265608</v>
+        <v>0.03232159999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>0.023282358</v>
+        <v>0.3354869999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>0.06432790799999999</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.024952208</v>
+        <v>0.01837625</v>
       </c>
     </row>
     <row r="14">
@@ -777,22 +736,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1432.1124</v>
+        <v>844.6276000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>1218.7174</v>
+        <v>1321.8376</v>
       </c>
       <c r="D14" t="n">
-        <v>1201.4274</v>
+        <v>462.52</v>
       </c>
       <c r="E14" t="n">
-        <v>1073.5724</v>
+        <v>2044.39</v>
       </c>
       <c r="F14" t="n">
-        <v>1634.1324</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1099.0524</v>
+        <v>646.3399999999999</v>
       </c>
     </row>
     <row r="15">
@@ -802,22 +758,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>40831.37280000001</v>
+        <v>29224.90480000001</v>
       </c>
       <c r="C15" t="n">
-        <v>35218.94780000002</v>
+        <v>37519.82480000001</v>
       </c>
       <c r="D15" t="n">
-        <v>39697.05780000002</v>
+        <v>15544.88</v>
       </c>
       <c r="E15" t="n">
-        <v>33003.0978</v>
+        <v>59785.87000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>37431.61280000001</v>
-      </c>
-      <c r="G15" t="n">
-        <v>33379.38280000001</v>
+        <v>23344.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>